<commit_message>
PROS-7528 SANOFIKH Kpi Update
</commit_message>
<xml_diff>
--- a/Projects/SANOFIKH/Data/Template.xlsx
+++ b/Projects/SANOFIKH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="90">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -651,6 +651,12 @@
     <t xml:space="preserve">GBD</t>
   </si>
   <si>
+    <t xml:space="preserve">GBD Platinuim </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBD Gold</t>
+  </si>
+  <si>
     <t xml:space="preserve">TELFAST OD 120MG</t>
   </si>
   <si>
@@ -735,6 +741,18 @@
     <t xml:space="preserve">Digestive Health</t>
   </si>
   <si>
+    <t xml:space="preserve">DOLIPRANE 1,000MG EFF TAB (NEW 2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENTEROGERMINA 5ML (NEW 2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enterogermina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELFAST 180MG (NEW 2019)</t>
+  </si>
+  <si>
     <t xml:space="preserve">SKUs</t>
   </si>
   <si>
@@ -762,10 +780,34 @@
     <t xml:space="preserve">WF-04</t>
   </si>
   <si>
+    <t xml:space="preserve">Telfast window Frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calcium Corbiere window Frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutritional</t>
+  </si>
+  <si>
     <t xml:space="preserve">Doliprane Counter Display</t>
   </si>
   <si>
     <t xml:space="preserve">CD-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doliprane &amp; Telfast Counter Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doliprane &amp; Telfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAIN &amp; Allergy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DOLIPRANE 1,00MG EFF TAB (NEW 2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TELFAST 120MG</t>
   </si>
 </sst>
 </file>
@@ -942,7 +984,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1085,13 +1127,6 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
       <right style="medium"/>
       <top style="medium"/>
       <bottom style="medium"/>
@@ -1148,7 +1183,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1257,14 +1292,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1329,55 +1364,47 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="18" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="21" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="20" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1385,19 +1412,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="23" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="22" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1405,7 +1428,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1413,11 +1436,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1507,11 +1526,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.10526315789474"/>
   </cols>
@@ -1768,19 +1787,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="11" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="11" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="12" width="3.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="12" width="9.10526315789474"/>
@@ -1819,27 +1838,39 @@
       <c r="G2" s="17" t="s">
         <v>36</v>
       </c>
+      <c r="H2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F3" s="23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1848,21 +1879,27 @@
         <v>23</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="27" t="n">
+        <v>46</v>
+      </c>
+      <c r="F4" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1871,21 +1908,27 @@
         <v>23</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C5" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="27" t="n">
+      <c r="F5" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1894,21 +1937,27 @@
         <v>23</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="27" t="n">
+        <v>52</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1917,21 +1966,27 @@
         <v>23</v>
       </c>
       <c r="B7" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="E7" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="27" t="n">
+      <c r="F7" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1940,21 +1995,27 @@
         <v>23</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="25" t="n">
         <v>3582910080282</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="27" t="n">
+        <v>57</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1963,21 +2024,27 @@
         <v>23</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C9" s="25" t="n">
         <v>3582910076117</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="27" t="n">
+        <v>57</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1986,21 +2053,27 @@
         <v>23</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C10" s="25" t="n">
         <v>3582910076155</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="27" t="n">
+        <v>57</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2009,21 +2082,27 @@
         <v>23</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C11" s="25" t="n">
         <v>3582910076148</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="27" t="n">
+        <v>57</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2032,22 +2111,28 @@
         <v>23</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C12" s="25" t="n">
         <v>3582910076124</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="27" t="n">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,21 +2140,114 @@
         <v>23</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="F13" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="27" t="n">
+        <v>65</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="25" t="n">
+        <v>3582910075820</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="25" t="n">
+        <v>3582910075455</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="25" t="n">
+        <v>8901083012138</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2098,12 +2276,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="11" width="4.82186234817814"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="11" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="11" width="4.39271255060729"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.39271255060729"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="11" width="3.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="12" width="9.10526315789474"/>
   </cols>
@@ -2131,7 +2309,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>32</v>
@@ -2326,17 +2504,17 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="11" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="100.368421052632"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="45.9554655870445"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="101.226720647773"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.39271255060729"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="12" width="3.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="12" width="9.10526315789474"/>
   </cols>
@@ -2395,19 +2573,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="11" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="20.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="11" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.39271255060729"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="12" width="3.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="12" width="9.10526315789474"/>
   </cols>
@@ -2445,50 +2624,68 @@
       <c r="G2" s="39" t="s">
         <v>36</v>
       </c>
+      <c r="H2" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="40" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F3" s="45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="46" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H3" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>68</v>
+      <c r="B4" s="48" t="s">
+        <v>74</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F4" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="47" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2496,92 +2693,175 @@
       <c r="A5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="47" t="s">
-        <v>70</v>
+      <c r="B5" s="48" t="s">
+        <v>76</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="49" t="n">
-        <v>1</v>
+        <v>53</v>
+      </c>
+      <c r="F5" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="47" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="47" t="s">
-        <v>72</v>
+      <c r="B6" s="48" t="s">
+        <v>78</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="32" t="n">
+        <v>65</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="47" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="32" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="47"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="54"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
+      <c r="B9" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
+      <c r="A10" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="47" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F11" s="33"/>
@@ -2654,19 +2934,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="11" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="11" width="7.60728744939271"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="12" width="3.96356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="12" width="9.10526315789474"/>
@@ -2681,7 +2961,7 @@
       <c r="F1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="55"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
@@ -2702,53 +2982,71 @@
       <c r="F2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="54" t="s">
         <v>36</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="57" t="s">
+      <c r="B3" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="C3" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="59" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="60" t="n">
-        <v>2</v>
+      <c r="D3" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3" s="47" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="56" t="n">
+        <v>8901083012138</v>
+      </c>
+      <c r="D4" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="E4" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="61" t="n">
+      <c r="F4" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="47" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="60" t="n">
+      <c r="I4" s="47" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2756,45 +3054,57 @@
       <c r="A5" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="E5" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="61" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" s="60" t="n">
-        <v>4</v>
+      <c r="F5" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="47" t="n">
+        <v>6</v>
+      </c>
+      <c r="I5" s="47" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="D6" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="61" t="n">
+      <c r="E6" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="47" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="60" t="n">
+      <c r="I6" s="47" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2802,114 +3112,144 @@
       <c r="A7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="E7" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="61" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="60" t="n">
-        <v>2</v>
+      <c r="F7" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="I7" s="47" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="58" t="n">
-        <v>3582910080282</v>
-      </c>
-      <c r="D8" s="57" t="s">
+      <c r="C8" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="61" t="n">
-        <v>4</v>
-      </c>
-      <c r="G8" s="60" t="n">
-        <v>4</v>
+      <c r="D8" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="47" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="56" t="n">
+        <v>3582910080282</v>
+      </c>
+      <c r="D9" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="58" t="n">
-        <v>3582910076117</v>
-      </c>
-      <c r="D9" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="61" t="n">
-        <v>4</v>
-      </c>
-      <c r="G9" s="60" t="n">
-        <v>4</v>
+      <c r="E9" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="47" t="n">
+        <v>6</v>
+      </c>
+      <c r="I9" s="47" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="56" t="n">
+        <v>3582910076117</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="58" t="n">
-        <v>3582910076155</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="61" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" s="60" t="n">
-        <v>4</v>
+      <c r="F10" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="47" t="n">
+        <v>6</v>
+      </c>
+      <c r="I10" s="47" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" s="58" t="n">
-        <v>3582910076148</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="61" t="n">
+      <c r="B11" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="56" t="n">
+        <v>3582910076155</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="47" t="n">
         <v>4</v>
       </c>
-      <c r="G11" s="60" t="n">
+      <c r="I11" s="47" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2917,22 +3257,28 @@
       <c r="A12" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="58" t="n">
-        <v>3582910076124</v>
-      </c>
-      <c r="D12" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="61" t="n">
+      <c r="B12" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="56" t="n">
+        <v>3582910076148</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="47" t="n">
         <v>4</v>
       </c>
-      <c r="G12" s="60" t="n">
+      <c r="I12" s="47" t="n">
         <v>4</v>
       </c>
     </row>
@@ -2940,68 +3286,231 @@
       <c r="A13" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="58" t="s">
+      <c r="B13" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="57" t="s">
+      <c r="C13" s="56" t="n">
+        <v>3582910076124</v>
+      </c>
+      <c r="D13" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="56" t="n">
+        <v>3582910075820</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="47" t="n">
+        <v>6</v>
+      </c>
+      <c r="I14" s="47" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="56" t="n">
+        <v>3582910075455</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="I15" s="47" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="C16" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="61" t="n">
+      <c r="D16" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="47" t="n">
         <v>4</v>
       </c>
-      <c r="G13" s="60" t="n">
+      <c r="I16" s="47" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="63" t="s">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="65" t="s">
+      <c r="B17" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="66" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="59" t="n">
+      <c r="F17" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="56" t="n">
+        <v>3582910080282</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="62" t="n">
+        <v>3582910075820</v>
+      </c>
+      <c r="D19" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="I19" s="47" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="56" t="n">
+        <v>8901083012139</v>
+      </c>
+      <c r="D20" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="47" t="n">
         <v>2</v>
       </c>
-      <c r="G14" s="67" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="58" t="n">
-        <v>3582910080282</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="61" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="60" t="n">
+      <c r="I20" s="47" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>